<commit_message>
Updates with the documentation
</commit_message>
<xml_diff>
--- a/Documentation/Kings Casino Risk Register V1.xlsx
+++ b/Documentation/Kings Casino Risk Register V1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daryl Atienza\Desktop\RPA\RPA.QA.FINAL PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daryl Atienza\Desktop\RPA\GIT.RPA.FINAL PROJECT\GroupProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6234E6-78DD-4230-B0E1-D19533B1EF4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8707797F-E700-4ABE-A71C-46C05A6CAC19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ACC8EF04-2AB8-46A2-BA29-9DB736E35C51}"/>
   </bookViews>
@@ -502,7 +502,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -609,30 +609,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -651,17 +631,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -704,19 +673,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
@@ -898,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -931,176 +887,149 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1109,49 +1038,67 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1470,17 +1417,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC43F2A3-C79A-4E52-8354-6FE0A2FACD36}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="35.140625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
@@ -1515,14 +1462,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="55">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1534,21 +1481,21 @@
       <c r="F2" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="73">
+      <c r="G2" s="41">
         <v>3</v>
       </c>
-      <c r="H2" s="84">
+      <c r="H2" s="44">
         <v>4</v>
       </c>
-      <c r="I2" s="90">
+      <c r="I2" s="80">
         <v>12</v>
       </c>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="53"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="12" t="s">
         <v>26</v>
       </c>
@@ -1558,15 +1505,15 @@
       <c r="F3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="91"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="53"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="12" t="s">
         <v>28</v>
       </c>
@@ -1576,33 +1523,33 @@
       <c r="F4" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="91"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="81"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="54"/>
+    <row r="5" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="92"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="82"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="55">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
         <v>2</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1614,21 +1561,21 @@
       <c r="F6" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="73">
+      <c r="G6" s="41">
         <v>2</v>
       </c>
-      <c r="H6" s="84">
+      <c r="H6" s="44">
         <v>4</v>
       </c>
-      <c r="I6" s="87">
+      <c r="I6" s="83">
         <v>8</v>
       </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="53"/>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="12" t="s">
         <v>30</v>
       </c>
@@ -1638,15 +1585,15 @@
       <c r="F7" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="88"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="84"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="53" t="s">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="58" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -1658,15 +1605,15 @@
       <c r="F8" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="88"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="84"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="54"/>
+    <row r="9" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="14" t="s">
         <v>32</v>
       </c>
@@ -1674,19 +1621,19 @@
         <v>61</v>
       </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="89"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="55">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
         <v>3</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -1698,21 +1645,21 @@
       <c r="F10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="76">
+      <c r="G10" s="67">
         <v>3</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="41">
         <v>3</v>
       </c>
-      <c r="I10" s="87">
+      <c r="I10" s="83">
         <v>9</v>
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="53"/>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="12" t="s">
         <v>33</v>
       </c>
@@ -1722,15 +1669,15 @@
       <c r="F11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="88"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="84"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="53"/>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="12" t="s">
         <v>35</v>
       </c>
@@ -1740,30 +1687,30 @@
       <c r="F12" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="88"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="84"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="54"/>
+    <row r="13" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="89"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="85"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="61">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="47">
         <v>4</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="50" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -1778,20 +1725,20 @@
       <c r="F14" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G14" s="41">
         <v>3</v>
       </c>
-      <c r="H14" s="84">
+      <c r="H14" s="44">
         <v>4</v>
       </c>
-      <c r="I14" s="90">
+      <c r="I14" s="80">
         <v>12</v>
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="65"/>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="48"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="13" t="s">
         <v>20</v>
       </c>
@@ -1804,14 +1751,14 @@
       <c r="F15" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="91"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="81"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="66"/>
+    <row r="16" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="15"/>
       <c r="D16" s="14" t="s">
         <v>38</v>
@@ -1822,19 +1769,19 @@
       <c r="F16" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="92"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="82"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="61">
+      <c r="A17" s="47">
         <v>5</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -1846,21 +1793,21 @@
       <c r="F17" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G17" s="41">
         <v>2</v>
       </c>
-      <c r="H17" s="84">
+      <c r="H17" s="44">
         <v>4</v>
       </c>
-      <c r="I17" s="87">
+      <c r="I17" s="83">
         <v>8</v>
       </c>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="53"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="12" t="s">
         <v>40</v>
       </c>
@@ -1870,15 +1817,15 @@
       <c r="F18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="74"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="88"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="84"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="53"/>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="12" t="s">
         <v>41</v>
       </c>
@@ -1888,50 +1835,50 @@
       <c r="F19" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="74"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="88"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="84"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="53"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="88"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="84"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="54"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="89"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="85"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="61">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="47">
         <v>6</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="59" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="10" t="s">
@@ -1940,55 +1887,55 @@
       <c r="F22" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G22" s="73">
+      <c r="G22" s="41">
         <v>3</v>
       </c>
-      <c r="H22" s="73">
+      <c r="H22" s="41">
         <v>3</v>
       </c>
-      <c r="I22" s="87">
+      <c r="I22" s="83">
         <v>9</v>
       </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="59"/>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="48"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="60"/>
       <c r="E23" s="12" t="s">
         <v>72</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="88"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="84"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63"/>
-      <c r="B24" s="66"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="60"/>
+    <row r="24" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="61"/>
       <c r="E24" s="14" t="s">
         <v>77</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="89"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="85"/>
       <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="61">
+      <c r="A25" s="47">
         <v>7</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -2000,21 +1947,21 @@
       <c r="F25" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="G25" s="73">
+      <c r="G25" s="41">
         <v>2</v>
       </c>
-      <c r="H25" s="84">
+      <c r="H25" s="44">
         <v>4</v>
       </c>
-      <c r="I25" s="87">
+      <c r="I25" s="83">
         <v>8</v>
       </c>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="53"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="12" t="s">
         <v>46</v>
       </c>
@@ -2024,15 +1971,15 @@
       <c r="F26" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="88"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="84"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="53"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="12" t="s">
         <v>44</v>
       </c>
@@ -2042,15 +1989,15 @@
       <c r="F27" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="74"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="88"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="84"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="63"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="54"/>
+    <row r="28" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="49"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="57"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
         <v>76</v>
@@ -2058,19 +2005,19 @@
       <c r="F28" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="75"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="89"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="85"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="61">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="47">
         <v>8</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="56" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="10" t="s">
@@ -2082,21 +2029,21 @@
       <c r="F29" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="73">
+      <c r="G29" s="41">
         <v>1</v>
       </c>
-      <c r="H29" s="73">
+      <c r="H29" s="41">
         <v>2</v>
       </c>
-      <c r="I29" s="79">
+      <c r="I29" s="86">
         <v>2</v>
       </c>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="63"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="54"/>
+    <row r="30" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="57"/>
       <c r="D30" s="14" t="s">
         <v>48</v>
       </c>
@@ -2104,16 +2051,16 @@
         <v>79</v>
       </c>
       <c r="F30" s="14"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="80"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="87"/>
       <c r="J30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="61">
+      <c r="A31" s="47">
         <v>9</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="50" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -2128,20 +2075,20 @@
       <c r="F31" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="G31" s="73">
+      <c r="G31" s="41">
         <v>1</v>
       </c>
-      <c r="H31" s="73">
+      <c r="H31" s="41">
         <v>2</v>
       </c>
-      <c r="I31" s="79">
+      <c r="I31" s="86">
         <v>2</v>
       </c>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="65"/>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="48"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="13" t="s">
         <v>21</v>
       </c>
@@ -2154,14 +2101,14 @@
       <c r="F32" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="81"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="88"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="63"/>
-      <c r="B33" s="66"/>
+    <row r="33" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="49"/>
+      <c r="B33" s="52"/>
       <c r="C33" s="15" t="s">
         <v>22</v>
       </c>
@@ -2170,16 +2117,16 @@
         <v>82</v>
       </c>
       <c r="F33" s="14"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="80"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="87"/>
       <c r="J33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="67">
+      <c r="A34" s="53">
         <v>10</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="50" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="17" t="s">
@@ -2194,20 +2141,20 @@
       <c r="F34" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G34" s="73">
+      <c r="G34" s="41">
         <v>1</v>
       </c>
-      <c r="H34" s="73">
+      <c r="H34" s="41">
         <v>2</v>
       </c>
-      <c r="I34" s="79">
+      <c r="I34" s="86">
         <v>2</v>
       </c>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="65"/>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="54"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="18" t="s">
         <v>23</v>
       </c>
@@ -2220,14 +2167,14 @@
       <c r="F35" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="81"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="88"/>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="69"/>
-      <c r="B36" s="66"/>
+      <c r="A36" s="55"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="19" t="s">
         <v>24</v>
       </c>
@@ -2240,9 +2187,9 @@
       <c r="F36" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="80"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="87"/>
       <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2264,25 +2211,25 @@
       <c r="F37" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="G37" s="82">
+      <c r="G37" s="35">
         <v>1</v>
       </c>
-      <c r="H37" s="82">
+      <c r="H37" s="35">
         <v>3</v>
       </c>
-      <c r="I37" s="83">
+      <c r="I37" s="89">
         <v>3</v>
       </c>
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="55">
+      <c r="A38" s="36">
         <v>12</v>
       </c>
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="16" t="s">
@@ -2294,20 +2241,20 @@
       <c r="F38" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G38" s="73">
+      <c r="G38" s="41">
         <v>1</v>
       </c>
-      <c r="H38" s="84">
+      <c r="H38" s="44">
         <v>4</v>
       </c>
-      <c r="I38" s="87">
+      <c r="I38" s="83">
         <v>4</v>
       </c>
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="71"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="7" t="s">
         <v>24</v>
       </c>
@@ -2320,55 +2267,55 @@
       <c r="F39" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="G39" s="74"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="88"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="84"/>
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="71"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="65"/>
       <c r="C40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="50"/>
+      <c r="E40" s="39"/>
       <c r="F40" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G40" s="74"/>
-      <c r="H40" s="85"/>
-      <c r="I40" s="88"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="84"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="71"/>
-      <c r="C41" s="50"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E41" s="50"/>
+      <c r="E41" s="39"/>
       <c r="F41" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G41" s="74"/>
-      <c r="H41" s="85"/>
-      <c r="I41" s="88"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="84"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="57"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="51"/>
+      <c r="A42" s="38"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="40"/>
       <c r="D42" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E42" s="51"/>
+      <c r="E42" s="40"/>
       <c r="F42" s="19"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="86"/>
-      <c r="I42" s="89"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="85"/>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
@@ -2414,35 +2361,30 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="I38:I42"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="H38:H42"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="H25:H28"/>
-    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:I16"/>
     <mergeCell ref="I17:I21"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="B22:B24"/>
@@ -2457,33 +2399,39 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="G17:G21"/>
     <mergeCell ref="H17:H21"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="I10:I13"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="I25:I28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I38:I42"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="H38:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2506,122 +2454,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-    </row>
-    <row r="2" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="76"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="72"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="27">
         <v>20</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="27">
         <v>15</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="27">
         <v>10</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="28">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="78"/>
+      <c r="B4" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="27">
         <v>16</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="27">
         <v>12</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="29">
         <v>8</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="28">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="78"/>
+      <c r="B5" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="27">
         <v>12</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="29">
         <v>9</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="29">
         <v>6</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="30">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="34" t="s">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="78"/>
+      <c r="B6" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="29">
         <v>8</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="29">
         <v>6</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="29">
         <v>4</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="30">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="31" t="s">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="79"/>
+      <c r="B7" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="31">
         <v>4</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="32">
         <v>3</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="32">
         <v>2</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="33">
         <v>1</v>
       </c>
     </row>

</xml_diff>